<commit_message>
Pull Data From DataFrame
</commit_message>
<xml_diff>
--- a/dog_data.xlsx
+++ b/dog_data.xlsx
@@ -985,7 +985,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1252,9 +1252,6 @@
       <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="D19">
-        <v>15214</v>
-      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">

</xml_diff>